<commit_message>
+added 3 new FX in the reaper project and added them to game music.fmod
</commit_message>
<xml_diff>
--- a/documentation/Audio-Asset-List.xlsx
+++ b/documentation/Audio-Asset-List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradm\Documents\SS-Asteroid-Hopefully-Last\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9898BE-594F-4C57-9225-B27212E39CFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0109A5-E0BE-41D2-B649-6F1FFA37F2E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F2467561-AE38-E34B-9F00-F00259329A33}"/>
+    <workbookView xWindow="-28920" yWindow="-5790" windowWidth="29040" windowHeight="15840" xr2:uid="{F2467561-AE38-E34B-9F00-F00259329A33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="58">
   <si>
     <t>Filename</t>
   </si>
@@ -174,19 +174,37 @@
     <t>asteroid whooshing past sound effect, heavy reverb, played at random intervals</t>
   </si>
   <si>
-    <t>Pew.mp3</t>
-  </si>
-  <si>
     <t>In progress</t>
   </si>
   <si>
-    <t>big-explosion.mp3</t>
-  </si>
-  <si>
-    <t>small-explosion.mp3</t>
-  </si>
-  <si>
     <t>Imported old version for testing sake -- will improve</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Proceed.wav</t>
+  </si>
+  <si>
+    <t>Skip.wav</t>
+  </si>
+  <si>
+    <t>Pew.wav</t>
+  </si>
+  <si>
+    <t>big-explosion.wav</t>
+  </si>
+  <si>
+    <t>small-explosion.wav</t>
+  </si>
+  <si>
+    <t>replace with its own heavier reverb version</t>
+  </si>
+  <si>
+    <t>Woosh.wav</t>
+  </si>
+  <si>
+    <t>I held the mic up to my desk fan</t>
   </si>
 </sst>
 </file>
@@ -564,7 +582,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -607,6 +625,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
       <c r="B3" t="s">
         <v>44</v>
       </c>
@@ -614,12 +635,15 @@
         <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>44</v>
@@ -628,10 +652,16 @@
         <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -639,10 +669,13 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -650,12 +683,12 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -664,12 +697,12 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -678,12 +711,12 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -692,7 +725,7 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -725,7 +758,7 @@
         <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -749,16 +782,13 @@
       <c r="C15" t="s">
         <v>18</v>
       </c>
-      <c r="D15" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
@@ -774,7 +804,7 @@
         <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
@@ -790,7 +820,7 @@
         <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
@@ -806,7 +836,7 @@
         <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.25">
@@ -838,7 +868,7 @@
         <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
@@ -862,7 +892,7 @@
         <v>32</v>
       </c>
       <c r="D29" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.25">
@@ -886,7 +916,7 @@
         <v>35</v>
       </c>
       <c r="D32" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
@@ -902,7 +932,7 @@
         <v>36</v>
       </c>
       <c r="D34" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
+Updated Audio Asset List
</commit_message>
<xml_diff>
--- a/documentation/Audio-Asset-List.xlsx
+++ b/documentation/Audio-Asset-List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradm\Documents\SS-Asteroid-Hopefully-Last\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8C4CA1-231E-4203-80C9-777990BB0AE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8102329-4BD3-4AE1-ADE4-4666ECA57241}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-5790" windowWidth="29040" windowHeight="15840" xr2:uid="{F2467561-AE38-E34B-9F00-F00259329A33}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F2467561-AE38-E34B-9F00-F00259329A33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="80">
   <si>
     <t>Filename</t>
   </si>
@@ -45,9 +45,6 @@
     <t>FX</t>
   </si>
   <si>
-    <t>Not Done</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>Dialogue</t>
   </si>
   <si>
-    <t>Game over/high scores music (slower, 8-bit/synth sounds)</t>
-  </si>
-  <si>
     <t>Interface</t>
   </si>
   <si>
@@ -159,9 +153,6 @@
     <t>I like the "Sphere of IO" sound in this video (4:51) and might try to mimic something like that: https://www.youtube.com/watch?v=-MmWeZHsQzs</t>
   </si>
   <si>
-    <t>Main menu/theme music (upbeat, fast-paced, 8-bit/synth sounds) -- while in game, ramp up intensity gradually</t>
-  </si>
-  <si>
     <t>Ambient/FX</t>
   </si>
   <si>
@@ -171,9 +162,6 @@
     <t>asteroid whooshing past sound effect, heavy reverb, played at random intervals</t>
   </si>
   <si>
-    <t>Imported old version for testing sake -- will improve</t>
-  </si>
-  <si>
     <t>Done</t>
   </si>
   <si>
@@ -268,6 +256,21 @@
   </si>
   <si>
     <t>22-Nate.wav, 23-Nate.wav, 24-Ken.wav</t>
+  </si>
+  <si>
+    <t>321.wav</t>
+  </si>
+  <si>
+    <t>Menus.wav</t>
+  </si>
+  <si>
+    <t>Game.wav</t>
+  </si>
+  <si>
+    <t>Game over/high scores/main menu music (slower, 8-bit/synth sounds)</t>
+  </si>
+  <si>
+    <t>theme music (upbeat, fast-paced, 8-bit/synth sounds) -- while in game, ramp up intensity gradually</t>
   </si>
 </sst>
 </file>
@@ -645,7 +648,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -661,7 +664,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -670,172 +673,181 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
         <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -843,241 +855,241 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D26" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D27" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C32" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D34" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D35" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>